<commit_message>
Bug Fix & Excel
Fixed a self-made bug and made more edits to the excel
</commit_message>
<xml_diff>
--- a/Resources/ExcelOutput/Test.xlsx
+++ b/Resources/ExcelOutput/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Study Name</t>
   </si>
@@ -33,9 +33,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>Reader ID</t>
-  </si>
-  <si>
     <t>No AVG</t>
   </si>
   <si>
@@ -69,12 +66,6 @@
     <t>Subject-ID</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>Pat-ID-type</t>
-  </si>
-  <si>
     <t>Study-ID</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>Baseline</t>
   </si>
   <si>
-    <t>StageName</t>
-  </si>
-  <si>
     <t>Subject-Gender</t>
   </si>
   <si>
@@ -99,12 +87,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Date-of-birth</t>
-  </si>
-  <si>
-    <t>A While Back</t>
-  </si>
-  <si>
     <t>Imaging-date</t>
   </si>
   <si>
@@ -114,21 +96,6 @@
     <t>Analysis-date</t>
   </si>
   <si>
-    <t>Machine-ID</t>
-  </si>
-  <si>
-    <t>GE Ultrasound</t>
-  </si>
-  <si>
-    <t>Probe-ID</t>
-  </si>
-  <si>
-    <t>Sonographer-ID</t>
-  </si>
-  <si>
-    <t>Interpreter-ID</t>
-  </si>
-  <si>
     <t>SDY-filename</t>
   </si>
   <si>
@@ -168,16 +135,7 @@
     <t>Confid-thresh</t>
   </si>
   <si>
-    <t>Trend-thresh</t>
-  </si>
-  <si>
-    <t>Trend-MSE-mm</t>
-  </si>
-  <si>
-    <t>Reproduc-round</t>
-  </si>
-  <si>
-    <t>Reading-number</t>
+    <t>40%</t>
   </si>
   <si>
     <t>Frame</t>
@@ -348,7 +306,7 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data -  - '!$H$2:$H$61</c:f>
+              <c:f>'Data -  - '!$E$2:$E$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -356,181 +314,181 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>4100</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>4700</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>5100</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0</c:v>
+                  <c:v>5900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,184 +500,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>21.91345287979836</c:v>
+                  <c:v>24.43969436047382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.91345287979836</c:v>
+                  <c:v>24.43969436047382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.08358376638763</c:v>
+                  <c:v>35.37809218763662</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.02002478747042</c:v>
+                  <c:v>35.75447597118858</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.03766814236533</c:v>
+                  <c:v>35.86596444558292</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.99147098561086</c:v>
+                  <c:v>35.77067467169414</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.7985423623186</c:v>
+                  <c:v>24.32861012297636</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.62926522160905</c:v>
+                  <c:v>24.17263638789651</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.88021213872462</c:v>
+                  <c:v>23.62047453353023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.9678322076362</c:v>
+                  <c:v>23.80186061288828</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.05690687389954</c:v>
+                  <c:v>24.1168750314678</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.05615446853632</c:v>
+                  <c:v>24.23211193523181</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.10976605216035</c:v>
+                  <c:v>24.18010957114192</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.08564044807481</c:v>
+                  <c:v>24.10757948972721</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.10178235875689</c:v>
+                  <c:v>24.08392740990866</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.12941326399377</c:v>
+                  <c:v>24.14567525699958</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.14907241581252</c:v>
+                  <c:v>24.1028518878085</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.08850434756592</c:v>
+                  <c:v>23.9924576483292</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21.1513260085595</c:v>
+                  <c:v>24.00425740433433</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.42346071963239</c:v>
+                  <c:v>24.45339043718502</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21.66992585186613</c:v>
+                  <c:v>24.69881576208547</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.70718614229494</c:v>
+                  <c:v>24.65253704067186</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21.69153025372675</c:v>
+                  <c:v>24.63571513688805</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.7179289540668</c:v>
+                  <c:v>24.60788832767959</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21.52676446576918</c:v>
+                  <c:v>24.47640249349195</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>21.37315692027423</c:v>
+                  <c:v>24.28760991527536</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21.24663171009657</c:v>
+                  <c:v>23.92145627821908</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>21.57245102763382</c:v>
+                  <c:v>24.30855878163534</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>21.82310625059071</c:v>
+                  <c:v>24.59270873725703</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21.86650593303795</c:v>
+                  <c:v>24.68925123200624</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21.80892241041149</c:v>
+                  <c:v>24.5941353818298</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>21.76726257772684</c:v>
+                  <c:v>24.49000530654262</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>21.67256967230992</c:v>
+                  <c:v>24.42649294350104</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>21.55137613777455</c:v>
+                  <c:v>24.2617118179304</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>21.36655722380631</c:v>
+                  <c:v>24.11673614185651</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>21.39573322365675</c:v>
+                  <c:v>24.01119243882869</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>21.65278700784421</c:v>
+                  <c:v>24.34851821951401</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>22.13934477863612</c:v>
+                  <c:v>24.83363151347939</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22.36799296766241</c:v>
+                  <c:v>36.53560547555191</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>22.20501132196329</c:v>
+                  <c:v>42.67062917156793</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>22.154981255147</c:v>
+                  <c:v>42.34139365264331</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>22.12579517521231</c:v>
+                  <c:v>42.17309016702146</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>22.11884655540978</c:v>
+                  <c:v>42.1786387102793</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>21.86455069753033</c:v>
+                  <c:v>34.35103130928262</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>21.61615275943661</c:v>
+                  <c:v>33.77425934140766</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>21.44038201542144</c:v>
+                  <c:v>33.80071594653138</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21.59357396211448</c:v>
+                  <c:v>33.15473112963728</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>22.07571985494613</c:v>
+                  <c:v>33.50400903098043</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>22.2231138020754</c:v>
+                  <c:v>32.46327461790699</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>21.92989754985318</c:v>
+                  <c:v>28.61209669111286</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>21.9128077761467</c:v>
+                  <c:v>32.86391900329808</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>21.86852446612423</c:v>
+                  <c:v>32.25205320169832</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>21.70539302176173</c:v>
+                  <c:v>32.86163025262231</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>21.56270404432714</c:v>
+                  <c:v>29.07232443926549</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>21.38379933797746</c:v>
+                  <c:v>29.76217726816773</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>21.75973361338127</c:v>
+                  <c:v>29.44278691163136</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>22.33743771380407</c:v>
+                  <c:v>29.84651132417257</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>22.31119137410756</c:v>
+                  <c:v>29.76194509308932</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>22.28856329598878</c:v>
+                  <c:v>34.23176934232991</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>22.20337564429612</c:v>
+                  <c:v>34.40217024278832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,53 +1104,50 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="20" customHeight="1">
@@ -1200,13 +1155,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2">
         <v>61</v>
@@ -1215,44 +1170,44 @@
         <v>6.1</v>
       </c>
       <c r="M2" s="2">
-        <v>21.69376118532629</v>
+        <v>28.67149048474273</v>
       </c>
       <c r="N2" s="2">
-        <v>20.88021213872462</v>
+        <v>23.62047453353023</v>
       </c>
       <c r="O2" s="2">
-        <v>22.36799296766241</v>
+        <v>42.67062917156793</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1274,36 +1229,30 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1311,101 +1260,95 @@
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="2" customFormat="1">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
         <v>10</v>
@@ -1413,80 +1356,37 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
       <c r="B23">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="2" customFormat="1">
-      <c r="A28" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1"/>
+    <row r="26" spans="1:2" s="2" customFormat="1"/>
+    <row r="28" spans="1:2" s="2" customFormat="1"/>
     <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="2" customFormat="1">
-      <c r="A30" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="2" customFormat="1">
-      <c r="A32" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="2" customFormat="1"/>
-    <row r="36" spans="1:1" s="2" customFormat="1"/>
-    <row r="38" spans="1:1" s="2" customFormat="1"/>
-    <row r="40" spans="1:1" s="2" customFormat="1"/>
-    <row r="42" spans="1:1" s="2" customFormat="1"/>
-    <row r="44" spans="1:1" s="2" customFormat="1"/>
-    <row r="46" spans="1:1" s="2" customFormat="1"/>
-    <row r="48" spans="1:1" s="2" customFormat="1"/>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1"/>
+    <row r="32" spans="1:2" s="2" customFormat="1"/>
+    <row r="34" s="2" customFormat="1"/>
+    <row r="36" s="2" customFormat="1"/>
+    <row r="38" s="2" customFormat="1"/>
+    <row r="40" s="2" customFormat="1"/>
+    <row r="42" s="2" customFormat="1"/>
+    <row r="44" s="2" customFormat="1"/>
+    <row r="46" s="2" customFormat="1"/>
+    <row r="48" s="2" customFormat="1"/>
     <row r="50" s="2" customFormat="1"/>
     <row r="52" s="2" customFormat="1"/>
     <row r="54" s="2" customFormat="1"/>
@@ -1512,28 +1412,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
@@ -1541,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>21.91345287979836</v>
+        <v>24.43969436047382</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -1558,7 +1458,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>21.91345287979836</v>
+        <v>24.43969436047382</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1575,16 +1475,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>22.08358376638763</v>
+        <v>35.37809218763662</v>
       </c>
       <c r="E4" s="2">
         <v>200</v>
       </c>
       <c r="G4" s="2">
-        <v>-0.7763764456586878</v>
+        <v>-44.75668830316231</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1592,16 +1492,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>22.02002478747042</v>
+        <v>35.75447597118858</v>
       </c>
       <c r="E5">
         <v>300</v>
       </c>
       <c r="G5">
-        <v>-0.4863309687278847</v>
+        <v>-46.29673941018715</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1">
@@ -1609,16 +1509,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>22.03766814236533</v>
+        <v>35.86596444558292</v>
       </c>
       <c r="E6" s="2">
         <v>400</v>
       </c>
       <c r="G6" s="2">
-        <v>-0.566844774524248</v>
+        <v>-46.75291726883764</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1626,16 +1526,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>21.99147098561086</v>
+        <v>35.77067467169414</v>
       </c>
       <c r="E7">
         <v>500</v>
       </c>
       <c r="G7">
-        <v>-0.3560283550038809</v>
+        <v>-46.36301970103953</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1">
@@ -1643,13 +1543,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>21.7985423623186</v>
+        <v>24.32861012297636</v>
       </c>
       <c r="E8" s="2">
         <v>600</v>
       </c>
       <c r="G8" s="2">
-        <v>0.5243834374713922</v>
+        <v>0.4545238408427645</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -1660,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>21.62926522160905</v>
+        <v>24.17263638789651</v>
       </c>
       <c r="E9">
         <v>700</v>
       </c>
       <c r="G9">
-        <v>1.296863893372558</v>
+        <v>1.092722227366366</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1677,13 +1577,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>20.88021213872462</v>
+        <v>23.62047453353023</v>
       </c>
       <c r="E10" s="2">
         <v>800</v>
       </c>
       <c r="G10" s="2">
-        <v>4.715097829362486</v>
+        <v>3.352005204567973</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -1694,13 +1594,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>20.9678322076362</v>
+        <v>23.80186061288828</v>
       </c>
       <c r="E11">
         <v>900</v>
       </c>
       <c r="G11">
-        <v>4.315251810607716</v>
+        <v>2.609827022293292</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1711,13 +1611,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>21.05690687389954</v>
+        <v>24.1168750314678</v>
       </c>
       <c r="E12" s="2">
         <v>1000</v>
       </c>
       <c r="G12" s="2">
-        <v>3.908767872398891</v>
+        <v>1.320881203523192</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -1728,13 +1628,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>21.05615446853632</v>
+        <v>24.23211193523181</v>
       </c>
       <c r="E13">
         <v>1100</v>
       </c>
       <c r="G13">
-        <v>3.912201404153756</v>
+        <v>0.8493658806868056</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1745,13 +1645,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>21.10976605216035</v>
+        <v>24.18010957114192</v>
       </c>
       <c r="E14" s="2">
         <v>1200</v>
       </c>
       <c r="G14" s="2">
-        <v>3.667549938599204</v>
+        <v>1.062144172112581</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
@@ -1762,13 +1662,13 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>21.08564044807481</v>
+        <v>24.10757948972721</v>
       </c>
       <c r="E15">
         <v>1300</v>
       </c>
       <c r="G15">
-        <v>3.777644884465944</v>
+        <v>1.358915810681068</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1779,13 +1679,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>21.10178235875689</v>
+        <v>24.08392740990866</v>
       </c>
       <c r="E16" s="2">
         <v>1400</v>
       </c>
       <c r="G16" s="2">
-        <v>3.703982779408274</v>
+        <v>1.455693124953879</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
@@ -1796,13 +1696,13 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>21.12941326399377</v>
+        <v>24.14567525699958</v>
       </c>
       <c r="E17">
         <v>1500</v>
       </c>
       <c r="G17">
-        <v>3.577891718412774</v>
+        <v>1.2030391998263</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1813,13 +1713,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>21.14907241581252</v>
+        <v>24.1028518878085</v>
       </c>
       <c r="E18" s="2">
         <v>1600</v>
       </c>
       <c r="G18" s="2">
-        <v>3.488179011216061</v>
+        <v>1.378259759295875</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1830,13 +1730,13 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>21.08850434756592</v>
+        <v>23.9924576483292</v>
       </c>
       <c r="E19">
         <v>1700</v>
       </c>
       <c r="G19">
-        <v>3.76457574603839</v>
+        <v>1.829960332351507</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1847,13 +1747,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>21.1513260085595</v>
+        <v>24.00425740433433</v>
       </c>
       <c r="E20" s="2">
         <v>1800</v>
       </c>
       <c r="G20" s="2">
-        <v>3.477894950738021</v>
+        <v>1.781679221176024</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1864,13 +1764,13 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>21.42346071963239</v>
+        <v>24.45339043718502</v>
       </c>
       <c r="E21">
         <v>1900</v>
       </c>
       <c r="G21">
-        <v>2.236033558260843</v>
+        <v>-0.0560402945683165</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1881,13 +1781,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>21.66992585186613</v>
+        <v>24.69881576208547</v>
       </c>
       <c r="E22" s="2">
         <v>2000</v>
       </c>
       <c r="G22" s="2">
-        <v>1.111312896548302</v>
+        <v>-1.060248126632605</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -1898,13 +1798,13 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>21.70718614229494</v>
+        <v>24.65253704067186</v>
       </c>
       <c r="E23">
         <v>2100</v>
       </c>
       <c r="G23">
-        <v>0.9412790336368231</v>
+        <v>-0.8708892879702687</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1915,13 +1815,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>21.69153025372675</v>
+        <v>24.63571513688805</v>
       </c>
       <c r="E24" s="2">
         <v>2200</v>
       </c>
       <c r="G24" s="2">
-        <v>1.012723222072394</v>
+        <v>-0.8020590336483917</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1932,13 +1832,13 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>21.7179289540668</v>
+        <v>24.60788832767959</v>
       </c>
       <c r="E25">
         <v>2300</v>
       </c>
       <c r="G25">
-        <v>0.8922552132887014</v>
+        <v>-0.6881999616074961</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1949,13 +1849,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>21.52676446576918</v>
+        <v>24.47640249349195</v>
       </c>
       <c r="E26" s="2">
         <v>2400</v>
       </c>
       <c r="G26" s="2">
-        <v>1.764616540123922</v>
+        <v>-0.1501988219521504</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
@@ -1966,13 +1866,13 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>21.37315692027423</v>
+        <v>24.28760991527536</v>
       </c>
       <c r="E27">
         <v>2500</v>
       </c>
       <c r="G27">
-        <v>2.465590258585979</v>
+        <v>0.6222845627906715</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1983,13 +1883,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>21.24663171009657</v>
+        <v>23.92145627821908</v>
       </c>
       <c r="E28" s="2">
         <v>2600</v>
       </c>
       <c r="G28" s="2">
-        <v>3.042976263756781</v>
+        <v>2.120476936458243</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
@@ -2000,13 +1900,13 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>21.57245102763382</v>
+        <v>24.30855878163534</v>
       </c>
       <c r="E29">
         <v>2700</v>
       </c>
       <c r="G29">
-        <v>1.556130172798597</v>
+        <v>0.5365679983729903</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2017,13 +1917,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>21.82310625059071</v>
+        <v>24.59270873725703</v>
       </c>
       <c r="E30" s="2">
         <v>2800</v>
       </c>
       <c r="G30" s="2">
-        <v>0.4122884225650451</v>
+        <v>-0.6260895677594104</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
@@ -2034,13 +1934,13 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>21.86650593303795</v>
+        <v>24.68925123200624</v>
       </c>
       <c r="E31">
         <v>2900</v>
       </c>
       <c r="G31">
-        <v>0.2142380163360625</v>
+        <v>-1.021112898760414</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2051,13 +1951,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>21.80892241041149</v>
+        <v>24.5941353818298</v>
       </c>
       <c r="E32" s="2">
         <v>3000</v>
       </c>
       <c r="G32" s="2">
-        <v>0.4770150553646331</v>
+        <v>-0.6319269753461642</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
@@ -2068,13 +1968,13 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>21.76726257772684</v>
+        <v>24.49000530654262</v>
       </c>
       <c r="E33">
         <v>3100</v>
       </c>
       <c r="G33">
-        <v>0.6671258193467577</v>
+        <v>-0.2058575092091545</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2085,13 +1985,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>21.67256967230992</v>
+        <v>24.42649294350104</v>
       </c>
       <c r="E34" s="2">
         <v>3200</v>
       </c>
       <c r="G34" s="2">
-        <v>1.099248068343017</v>
+        <v>0.05401629324027432</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
@@ -2102,13 +2002,13 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>21.55137613777455</v>
+        <v>24.2617118179304</v>
       </c>
       <c r="E35">
         <v>3300</v>
       </c>
       <c r="G35">
-        <v>1.652303468604007</v>
+        <v>0.7282519164039339</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2119,13 +2019,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>21.36655722380631</v>
+        <v>24.11673614185651</v>
       </c>
       <c r="E36" s="2">
         <v>3400</v>
       </c>
       <c r="G36" s="2">
-        <v>2.495707358360793</v>
+        <v>1.321449498728691</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
@@ -2136,13 +2036,13 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>21.39573322365675</v>
+        <v>24.01119243882869</v>
       </c>
       <c r="E37">
         <v>3500</v>
       </c>
       <c r="G37">
-        <v>2.362565402090917</v>
+        <v>1.753303111425727</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2153,13 +2053,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>21.65278700784421</v>
+        <v>24.34851821951401</v>
       </c>
       <c r="E38" s="2">
         <v>3600</v>
       </c>
       <c r="G38" s="2">
-        <v>1.189524413993436</v>
+        <v>0.3730657986757049</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
@@ -2170,13 +2070,13 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>22.13934477863612</v>
+        <v>24.83363151347939</v>
       </c>
       <c r="E39">
         <v>3700</v>
       </c>
       <c r="G39">
-        <v>-1.030836628425626</v>
+        <v>-1.611874302498192</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2187,16 +2087,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>22.36799296766241</v>
+        <v>36.53560547555191</v>
       </c>
       <c r="E40" s="2">
         <v>3800</v>
       </c>
       <c r="G40" s="2">
-        <v>-2.074251330255104</v>
+        <v>-49.49289028196992</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2204,16 +2104,16 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>22.20501132196329</v>
+        <v>42.67062917156793</v>
       </c>
       <c r="E41">
         <v>3900</v>
       </c>
       <c r="G41">
-        <v>-1.330499779127505</v>
+        <v>-74.59559249062831</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1">
@@ -2221,16 +2121,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>22.154981255147</v>
+        <v>42.34139365264331</v>
       </c>
       <c r="E42" s="2">
         <v>4000</v>
       </c>
       <c r="G42" s="2">
-        <v>-1.102192231746815</v>
+        <v>-73.24845813588331</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2238,16 +2138,16 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>22.12579517521231</v>
+        <v>42.17309016702146</v>
       </c>
       <c r="E43">
         <v>4100</v>
       </c>
       <c r="G43">
-        <v>-0.9690042759518827</v>
+        <v>-72.55981005731304</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1">
@@ -2255,16 +2155,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>22.11884655540978</v>
+        <v>42.1786387102793</v>
       </c>
       <c r="E44" s="2">
         <v>4200</v>
       </c>
       <c r="G44" s="2">
-        <v>-0.9372948970573561</v>
+        <v>-72.58251305505107</v>
       </c>
       <c r="H44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2272,16 +2172,16 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>21.86455069753033</v>
+        <v>34.35103130928262</v>
       </c>
       <c r="E45">
         <v>4300</v>
       </c>
       <c r="G45">
-        <v>0.2231605513575274</v>
+        <v>-40.55425899612867</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1">
@@ -2289,13 +2189,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>21.61615275943661</v>
+        <v>33.77425934140766</v>
       </c>
       <c r="E46" s="2">
         <v>4400</v>
       </c>
       <c r="G46" s="2">
-        <v>1.356701392484934</v>
+        <v>-38.19427871418303</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
@@ -2306,13 +2206,13 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>21.44038201542144</v>
+        <v>33.80071594653138</v>
       </c>
       <c r="E47">
         <v>4500</v>
       </c>
       <c r="G47">
-        <v>2.158814801902067</v>
+        <v>-38.30253131641896</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2323,13 +2223,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>21.59357396211448</v>
+        <v>33.15473112963728</v>
       </c>
       <c r="E48" s="2">
         <v>4600</v>
       </c>
       <c r="G48" s="2">
-        <v>1.459737629840941</v>
+        <v>-35.65935252962183</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
@@ -2340,13 +2240,13 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>22.07571985494613</v>
+        <v>33.50400903098043</v>
       </c>
       <c r="E49">
         <v>4700</v>
       </c>
       <c r="G49">
-        <v>-0.7404902186699819</v>
+        <v>-37.08849438463632</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2357,13 +2257,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>22.2231138020754</v>
+        <v>32.46327461790699</v>
       </c>
       <c r="E50" s="2">
         <v>4800</v>
       </c>
       <c r="G50" s="2">
-        <v>-1.413108760064479</v>
+        <v>-32.8301170181967</v>
       </c>
       <c r="H50" s="2">
         <v>0</v>
@@ -2374,13 +2274,13 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>21.92989754985318</v>
+        <v>28.61209669111286</v>
       </c>
       <c r="E51">
         <v>4900</v>
       </c>
       <c r="G51">
-        <v>-0.07504371923957896</v>
+        <v>-17.07223612987179</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -2391,13 +2291,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>21.9128077761467</v>
+        <v>32.86391900329808</v>
       </c>
       <c r="E52" s="2">
         <v>5000</v>
       </c>
       <c r="G52" s="2">
-        <v>0.002943870394163057</v>
+        <v>-34.4694353316002</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
@@ -2408,13 +2308,13 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>21.86852446612423</v>
+        <v>32.25205320169832</v>
       </c>
       <c r="E53">
         <v>5100</v>
       </c>
       <c r="G53">
-        <v>0.2050266287133335</v>
+        <v>-31.96586146289696</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -2425,13 +2325,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>21.70539302176173</v>
+        <v>32.86163025262231</v>
       </c>
       <c r="E54" s="2">
         <v>5200</v>
       </c>
       <c r="G54" s="2">
-        <v>0.9494617720808436</v>
+        <v>-34.46007044085317</v>
       </c>
       <c r="H54" s="2">
         <v>0</v>
@@ -2442,13 +2342,13 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>21.56270404432714</v>
+        <v>29.07232443926549</v>
       </c>
       <c r="E55">
         <v>5300</v>
       </c>
       <c r="G55">
-        <v>1.600609622751763</v>
+        <v>-18.95535193878692</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -2459,13 +2359,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>21.38379933797746</v>
+        <v>29.76217726816773</v>
       </c>
       <c r="E56" s="2">
         <v>5400</v>
       </c>
       <c r="G56" s="2">
-        <v>2.417024577213833</v>
+        <v>-21.77802565445311</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -2476,13 +2376,13 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>21.75973361338127</v>
+        <v>29.44278691163136</v>
       </c>
       <c r="E57">
         <v>5500</v>
       </c>
       <c r="G57">
-        <v>0.7014835464784573</v>
+        <v>-20.471174791977</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2493,13 +2393,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>22.33743771380407</v>
+        <v>29.84651132417257</v>
       </c>
       <c r="E58" s="2">
         <v>5600</v>
       </c>
       <c r="G58" s="2">
-        <v>-1.934815276859323</v>
+        <v>-22.12309566539905</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
@@ -2510,13 +2410,13 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>22.31119137410756</v>
+        <v>29.76194509308932</v>
       </c>
       <c r="E59">
         <v>5700</v>
       </c>
       <c r="G59">
-        <v>-1.815042551673208</v>
+        <v>-21.77707566271022</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2527,16 +2427,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>22.28856329598878</v>
+        <v>34.23176934232991</v>
       </c>
       <c r="E60" s="2">
         <v>5800</v>
       </c>
       <c r="G60" s="2">
-        <v>-1.711781425994386</v>
+        <v>-40.06627430534797</v>
       </c>
       <c r="H60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2544,24 +2444,24 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>22.20337564429612</v>
+        <v>34.40217024278832</v>
       </c>
       <c r="E61">
         <v>5900</v>
       </c>
       <c r="G61">
-        <v>-1.323035516529825</v>
+        <v>-40.76350438500883</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="B62">
-        <v>22.13261122998172</v>
+        <v>29.95937605115229</v>
       </c>
       <c r="G62">
-        <v>-1.000108706672122</v>
+        <v>-22.58490474252993</v>
       </c>
       <c r="H62">
         <v>0</v>

</xml_diff>

<commit_message>
File bsl1 converted to AVI
Used MicroDicom viewer to convert files to AVI. Temporary way to see the files.
measured ratio to be 16.8pix/mm using measuring tool on the viewer. Not sure if we want to hardcode that or not.
Also theese are big so commiting is interesting.
</commit_message>
<xml_diff>
--- a/Resources/ExcelOutput/Test.xlsx
+++ b/Resources/ExcelOutput/Test.xlsx
@@ -60,7 +60,7 @@
     <t>Report-date</t>
   </si>
   <si>
-    <t>Apr 23, 2020  (04-23-20)</t>
+    <t>Apr 24, 2020  (04-24-20)</t>
   </si>
   <si>
     <t>Subject-ID</t>
@@ -306,10 +306,10 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data -  - '!$E$2:$E$61</c:f>
+              <c:f>'Data -  - '!$E$2:$E$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -486,198 +486,192 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data -  - '!$B$2:$B$61</c:f>
+              <c:f>'Data -  - '!$B$2:$B$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
-                  <c:v>24.43969436047382</c:v>
+                  <c:v>23.2118205787922</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.43969436047382</c:v>
+                  <c:v>23.308371827441</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.37809218763662</c:v>
+                  <c:v>23.19129694891313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.75447597118858</c:v>
+                  <c:v>23.22306519177809</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.86596444558292</c:v>
+                  <c:v>23.2143264470056</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.77067467169414</c:v>
+                  <c:v>22.92541707830276</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.32861012297636</c:v>
+                  <c:v>22.78462230666184</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.17263638789651</c:v>
+                  <c:v>22.22535623347705</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.62047453353023</c:v>
+                  <c:v>22.11821697057012</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.80186061288828</c:v>
+                  <c:v>22.5279880816139</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.1168750314678</c:v>
+                  <c:v>22.67748200797255</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.23211193523181</c:v>
+                  <c:v>22.64940157532551</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.18010957114192</c:v>
+                  <c:v>22.5755043271278</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.10757948972721</c:v>
+                  <c:v>22.61933782032324</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.08392740990866</c:v>
+                  <c:v>22.58831455379097</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.14567525699958</c:v>
+                  <c:v>22.50702376342007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.1028518878085</c:v>
+                  <c:v>22.33400680195176</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.9924576483292</c:v>
+                  <c:v>22.33344330238226</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.00425740433433</c:v>
+                  <c:v>22.87712133434471</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.45339043718502</c:v>
+                  <c:v>23.09188549568665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.69881576208547</c:v>
+                  <c:v>23.03772487117502</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24.65253704067186</c:v>
+                  <c:v>22.99641650694106</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>24.63571513688805</c:v>
+                  <c:v>23.04332170796958</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24.60788832767959</c:v>
+                  <c:v>22.92175645988742</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.47640249349195</c:v>
+                  <c:v>22.63749334457248</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24.28760991527536</c:v>
+                  <c:v>22.5374723983163</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.92145627821908</c:v>
+                  <c:v>22.89247154483127</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24.30855878163534</c:v>
+                  <c:v>23.19119522173441</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.59270873725703</c:v>
+                  <c:v>23.33982450103375</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24.68925123200624</c:v>
+                  <c:v>23.24003331922056</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>24.5941353818298</c:v>
+                  <c:v>23.21471295136624</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>24.49000530654262</c:v>
+                  <c:v>23.09454674409804</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>24.42649294350104</c:v>
+                  <c:v>22.85324718841161</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>24.2617118179304</c:v>
+                  <c:v>22.70091789226527</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>24.11673614185651</c:v>
+                  <c:v>22.67004812593076</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>24.01119243882869</c:v>
+                  <c:v>22.90463075172562</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>24.34851821951401</c:v>
+                  <c:v>23.49328170570378</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>24.83363151347939</c:v>
+                  <c:v>23.66716218425726</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>36.53560547555191</c:v>
+                  <c:v>23.40193732281057</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42.67062917156793</c:v>
+                  <c:v>23.38562308358792</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42.34139365264331</c:v>
+                  <c:v>23.44678212339621</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42.17309016702146</c:v>
+                  <c:v>23.45234185595259</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.1786387102793</c:v>
+                  <c:v>26.71173362577946</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>34.35103130928262</c:v>
+                  <c:v>26.54481049203902</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>33.77425934140766</c:v>
+                  <c:v>26.2876480333941</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>33.80071594653138</c:v>
+                  <c:v>23.13264664306285</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>33.15473112963728</c:v>
+                  <c:v>23.82215554246476</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>33.50400903098043</c:v>
+                  <c:v>23.84729001493749</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>32.46327461790699</c:v>
+                  <c:v>26.53655605818091</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>28.61209669111286</c:v>
+                  <c:v>23.56219569603061</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>32.86391900329808</c:v>
+                  <c:v>23.47901848676972</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>32.25205320169832</c:v>
+                  <c:v>23.30782017760622</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>32.86163025262231</c:v>
+                  <c:v>23.04100986254222</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>29.07232443926549</c:v>
+                  <c:v>23.03426223551625</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>29.76217726816773</c:v>
+                  <c:v>23.67532550030654</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>29.44278691163136</c:v>
+                  <c:v>23.78346015101411</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>29.84651132417257</c:v>
+                  <c:v>23.78624119172401</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>29.76194509308932</c:v>
+                  <c:v>23.75771675344369</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>34.23176934232991</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>34.40217024278832</c:v>
+                  <c:v>23.69933032256922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1164,19 +1158,19 @@
         <v>27</v>
       </c>
       <c r="J2" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="2">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="M2" s="2">
-        <v>28.67149048474273</v>
+        <v>23.31286041612941</v>
       </c>
       <c r="N2" s="2">
-        <v>23.62047453353023</v>
+        <v>22.11821697057012</v>
       </c>
       <c r="O2" s="2">
-        <v>42.67062917156793</v>
+        <v>26.71173362577946</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1366,7 +1360,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="B23">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1"/>
@@ -1401,7 +1395,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1441,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>24.43969436047382</v>
+        <v>23.2118205787922</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -1458,13 +1452,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>24.43969436047382</v>
+        <v>23.308371827441</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-0.4159572417900726</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1475,16 +1469,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>35.37809218763662</v>
+        <v>23.19129694891313</v>
       </c>
       <c r="E4" s="2">
         <v>200</v>
       </c>
       <c r="G4" s="2">
-        <v>-44.75668830316231</v>
+        <v>0.08841887179593702</v>
       </c>
       <c r="H4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1492,16 +1486,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>35.75447597118858</v>
+        <v>23.22306519177809</v>
       </c>
       <c r="E5">
         <v>300</v>
       </c>
       <c r="G5">
-        <v>-46.29673941018715</v>
+        <v>-0.04844347709704562</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1">
@@ -1509,16 +1503,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>35.86596444558292</v>
+        <v>23.2143264470056</v>
       </c>
       <c r="E6" s="2">
         <v>400</v>
       </c>
       <c r="G6" s="2">
-        <v>-46.75291726883764</v>
+        <v>-0.01079565562250835</v>
       </c>
       <c r="H6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1526,16 +1520,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>35.77067467169414</v>
+        <v>22.92541707830276</v>
       </c>
       <c r="E7">
         <v>500</v>
       </c>
       <c r="G7">
-        <v>-46.36301970103953</v>
+        <v>1.233869181080556</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1">
@@ -1543,13 +1537,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>24.32861012297636</v>
+        <v>22.78462230666184</v>
       </c>
       <c r="E8" s="2">
         <v>600</v>
       </c>
       <c r="G8" s="2">
-        <v>0.4545238408427645</v>
+        <v>1.840434147249383</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -1560,13 +1554,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>24.17263638789651</v>
+        <v>22.22535623347705</v>
       </c>
       <c r="E9">
         <v>700</v>
       </c>
       <c r="G9">
-        <v>1.092722227366366</v>
+        <v>4.249836164150112</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1577,13 +1571,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>23.62047453353023</v>
+        <v>22.11821697057012</v>
       </c>
       <c r="E10" s="2">
         <v>800</v>
       </c>
       <c r="G10" s="2">
-        <v>3.352005204567973</v>
+        <v>4.711408157364692</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -1594,13 +1588,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>23.80186061288828</v>
+        <v>22.5279880816139</v>
       </c>
       <c r="E11">
         <v>900</v>
       </c>
       <c r="G11">
-        <v>2.609827022293292</v>
+        <v>2.946052830526747</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1611,13 +1605,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>24.1168750314678</v>
+        <v>22.67748200797255</v>
       </c>
       <c r="E12" s="2">
         <v>1000</v>
       </c>
       <c r="G12" s="2">
-        <v>1.320881203523192</v>
+        <v>2.302010602769557</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -1628,13 +1622,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>24.23211193523181</v>
+        <v>22.64940157532551</v>
       </c>
       <c r="E13">
         <v>1100</v>
       </c>
       <c r="G13">
-        <v>0.8493658806868056</v>
+        <v>2.422985312839064</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1645,13 +1639,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>24.18010957114192</v>
+        <v>22.5755043271278</v>
       </c>
       <c r="E14" s="2">
         <v>1200</v>
       </c>
       <c r="G14" s="2">
-        <v>1.062144172112581</v>
+        <v>2.741345727296257</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
@@ -1662,13 +1656,13 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>24.10757948972721</v>
+        <v>22.61933782032324</v>
       </c>
       <c r="E15">
         <v>1300</v>
       </c>
       <c r="G15">
-        <v>1.358915810681068</v>
+        <v>2.552504472700808</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1679,13 +1673,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>24.08392740990866</v>
+        <v>22.58831455379097</v>
       </c>
       <c r="E16" s="2">
         <v>1400</v>
       </c>
       <c r="G16" s="2">
-        <v>1.455693124953879</v>
+        <v>2.686157351961001</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
@@ -1696,13 +1690,13 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>24.14567525699958</v>
+        <v>22.50702376342007</v>
       </c>
       <c r="E17">
         <v>1500</v>
       </c>
       <c r="G17">
-        <v>1.2030391998263</v>
+        <v>3.036370253594318</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1713,13 +1707,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>24.1028518878085</v>
+        <v>22.33400680195176</v>
       </c>
       <c r="E18" s="2">
         <v>1600</v>
       </c>
       <c r="G18" s="2">
-        <v>1.378259759295875</v>
+        <v>3.781753240167916</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1730,13 +1724,13 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>23.9924576483292</v>
+        <v>22.33344330238226</v>
       </c>
       <c r="E19">
         <v>1700</v>
       </c>
       <c r="G19">
-        <v>1.829960332351507</v>
+        <v>3.784180880721095</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1747,13 +1741,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>24.00425740433433</v>
+        <v>22.87712133434471</v>
       </c>
       <c r="E20" s="2">
         <v>1800</v>
       </c>
       <c r="G20" s="2">
-        <v>1.781679221176024</v>
+        <v>1.44193448037114</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1764,13 +1758,13 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>24.45339043718502</v>
+        <v>23.09188549568665</v>
       </c>
       <c r="E21">
         <v>1900</v>
       </c>
       <c r="G21">
-        <v>-0.0560402945683165</v>
+        <v>0.5166983033425901</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1781,13 +1775,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>24.69881576208547</v>
+        <v>23.03772487117502</v>
       </c>
       <c r="E22" s="2">
         <v>2000</v>
       </c>
       <c r="G22" s="2">
-        <v>-1.060248126632605</v>
+        <v>0.7500303865705463</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -1798,13 +1792,13 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>24.65253704067186</v>
+        <v>22.99641650694106</v>
       </c>
       <c r="E23">
         <v>2100</v>
       </c>
       <c r="G23">
-        <v>-0.8708892879702687</v>
+        <v>0.9279930073556704</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1815,13 +1809,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>24.63571513688805</v>
+        <v>23.04332170796958</v>
       </c>
       <c r="E24" s="2">
         <v>2200</v>
       </c>
       <c r="G24" s="2">
-        <v>-0.8020590336483917</v>
+        <v>0.7259183752978364</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1832,13 +1826,13 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>24.60788832767959</v>
+        <v>22.92175645988742</v>
       </c>
       <c r="E25">
         <v>2300</v>
       </c>
       <c r="G25">
-        <v>-0.6881999616074961</v>
+        <v>1.24963967354546</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1849,13 +1843,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>24.47640249349195</v>
+        <v>22.63749334457248</v>
       </c>
       <c r="E26" s="2">
         <v>2400</v>
       </c>
       <c r="G26" s="2">
-        <v>-0.1501988219521504</v>
+        <v>2.474287754681571</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
@@ -1866,13 +1860,13 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>24.28760991527536</v>
+        <v>22.5374723983163</v>
       </c>
       <c r="E27">
         <v>2500</v>
       </c>
       <c r="G27">
-        <v>0.6222845627906715</v>
+        <v>2.905192973497421</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1883,13 +1877,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>23.92145627821908</v>
+        <v>22.89247154483127</v>
       </c>
       <c r="E28" s="2">
         <v>2600</v>
       </c>
       <c r="G28" s="2">
-        <v>2.120476936458243</v>
+        <v>1.375803474255267</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
@@ -1900,13 +1894,13 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>24.30855878163534</v>
+        <v>23.19119522173441</v>
       </c>
       <c r="E29">
         <v>2700</v>
       </c>
       <c r="G29">
-        <v>0.5365679983729903</v>
+        <v>0.08885712771977095</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1917,13 +1911,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>24.59270873725703</v>
+        <v>23.33982450103375</v>
       </c>
       <c r="E30" s="2">
         <v>2800</v>
       </c>
       <c r="G30" s="2">
-        <v>-0.6260895677594104</v>
+        <v>-0.5514600709885998</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
@@ -1934,13 +1928,13 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>24.68925123200624</v>
+        <v>23.24003331922056</v>
       </c>
       <c r="E31">
         <v>2900</v>
       </c>
       <c r="G31">
-        <v>-1.021112898760414</v>
+        <v>-0.1215447118100792</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1951,13 +1945,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>24.5941353818298</v>
+        <v>23.21471295136624</v>
       </c>
       <c r="E32" s="2">
         <v>3000</v>
       </c>
       <c r="G32" s="2">
-        <v>-0.6319269753461642</v>
+        <v>-0.01246077430346726</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
@@ -1968,13 +1962,13 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>24.49000530654262</v>
+        <v>23.09454674409804</v>
       </c>
       <c r="E33">
         <v>3100</v>
       </c>
       <c r="G33">
-        <v>-0.2058575092091545</v>
+        <v>0.5052332465524128</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1985,13 +1979,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>24.42649294350104</v>
+        <v>22.85324718841161</v>
       </c>
       <c r="E34" s="2">
         <v>3200</v>
       </c>
       <c r="G34" s="2">
-        <v>0.05401629324027432</v>
+        <v>1.544787877208579</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
@@ -2002,13 +1996,13 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>24.2617118179304</v>
+        <v>22.70091789226527</v>
       </c>
       <c r="E35">
         <v>3300</v>
       </c>
       <c r="G35">
-        <v>0.7282519164039339</v>
+        <v>2.201045302726989</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2019,13 +2013,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>24.11673614185651</v>
+        <v>22.67004812593076</v>
       </c>
       <c r="E36" s="2">
         <v>3400</v>
       </c>
       <c r="G36" s="2">
-        <v>1.321449498728691</v>
+        <v>2.33403688014216</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
@@ -2036,13 +2030,13 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>24.01119243882869</v>
+        <v>22.90463075172562</v>
       </c>
       <c r="E37">
         <v>3500</v>
       </c>
       <c r="G37">
-        <v>1.753303111425727</v>
+        <v>1.323419789601687</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2053,13 +2047,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>24.34851821951401</v>
+        <v>23.49328170570378</v>
       </c>
       <c r="E38" s="2">
         <v>3600</v>
       </c>
       <c r="G38" s="2">
-        <v>0.3730657986757049</v>
+        <v>-1.212576695378854</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
@@ -2070,13 +2064,13 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>24.83363151347939</v>
+        <v>23.66716218425726</v>
       </c>
       <c r="E39">
         <v>3700</v>
       </c>
       <c r="G39">
-        <v>-1.611874302498192</v>
+        <v>-1.961679842903381</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2087,16 +2081,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>36.53560547555191</v>
+        <v>23.40193732281057</v>
       </c>
       <c r="E40" s="2">
         <v>3800</v>
       </c>
       <c r="G40" s="2">
-        <v>-49.49289028196992</v>
+        <v>-0.8190514112110548</v>
       </c>
       <c r="H40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2104,16 +2098,16 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>42.67062917156793</v>
+        <v>23.38562308358792</v>
       </c>
       <c r="E41">
         <v>3900</v>
       </c>
       <c r="G41">
-        <v>-74.59559249062831</v>
+        <v>-0.7487672248962701</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1">
@@ -2121,16 +2115,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>42.34139365264331</v>
+        <v>23.44678212339621</v>
       </c>
       <c r="E42" s="2">
         <v>4000</v>
       </c>
       <c r="G42" s="2">
-        <v>-73.24845813588331</v>
+        <v>-1.012249529529342</v>
       </c>
       <c r="H42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2138,16 +2132,16 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>42.17309016702146</v>
+        <v>23.45234185595259</v>
       </c>
       <c r="E43">
         <v>4100</v>
       </c>
       <c r="G43">
-        <v>-72.55981005731304</v>
+        <v>-1.036201690186046</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1">
@@ -2155,16 +2149,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>42.1786387102793</v>
+        <v>26.71173362577946</v>
       </c>
       <c r="E44" s="2">
         <v>4200</v>
       </c>
       <c r="G44" s="2">
-        <v>-72.58251305505107</v>
+        <v>-15.07814966562773</v>
       </c>
       <c r="H44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2172,16 +2166,16 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>34.35103130928262</v>
+        <v>26.54481049203902</v>
       </c>
       <c r="E45">
         <v>4300</v>
       </c>
       <c r="G45">
-        <v>-40.55425899612867</v>
+        <v>-14.35901980171284</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1">
@@ -2189,13 +2183,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>33.77425934140766</v>
+        <v>26.2876480333941</v>
       </c>
       <c r="E46" s="2">
         <v>4400</v>
       </c>
       <c r="G46" s="2">
-        <v>-38.19427871418303</v>
+        <v>-13.25112540897451</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
@@ -2206,13 +2200,13 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>33.80071594653138</v>
+        <v>23.13264664306285</v>
       </c>
       <c r="E47">
         <v>4500</v>
       </c>
       <c r="G47">
-        <v>-38.30253131641896</v>
+        <v>0.3410931747494602</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2223,13 +2217,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>33.15473112963728</v>
+        <v>23.82215554246476</v>
       </c>
       <c r="E48" s="2">
         <v>4600</v>
       </c>
       <c r="G48" s="2">
-        <v>-35.65935252962183</v>
+        <v>-2.629414446836662</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
@@ -2240,13 +2234,13 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>33.50400903098043</v>
+        <v>23.84729001493749</v>
       </c>
       <c r="E49">
         <v>4700</v>
       </c>
       <c r="G49">
-        <v>-37.08849438463632</v>
+        <v>-2.737697519193711</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2257,13 +2251,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>32.46327461790699</v>
+        <v>26.53655605818091</v>
       </c>
       <c r="E50" s="2">
         <v>4800</v>
       </c>
       <c r="G50" s="2">
-        <v>-32.8301170181967</v>
+        <v>-14.32345846420337</v>
       </c>
       <c r="H50" s="2">
         <v>0</v>
@@ -2274,13 +2268,13 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>28.61209669111286</v>
+        <v>23.56219569603061</v>
       </c>
       <c r="E51">
         <v>4900</v>
       </c>
       <c r="G51">
-        <v>-17.07223612987179</v>
+        <v>-1.509468488475806</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -2291,13 +2285,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>32.86391900329808</v>
+        <v>23.47901848676972</v>
       </c>
       <c r="E52" s="2">
         <v>5000</v>
       </c>
       <c r="G52" s="2">
-        <v>-34.4694353316002</v>
+        <v>-1.151128611693898</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
@@ -2308,13 +2302,13 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>32.25205320169832</v>
+        <v>23.30782017760622</v>
       </c>
       <c r="E53">
         <v>5100</v>
       </c>
       <c r="G53">
-        <v>-31.96586146289696</v>
+        <v>-0.4135806516690892</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -2325,13 +2319,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>32.86163025262231</v>
+        <v>23.04100986254222</v>
       </c>
       <c r="E54" s="2">
         <v>5200</v>
       </c>
       <c r="G54" s="2">
-        <v>-34.46007044085317</v>
+        <v>0.7358781516950097</v>
       </c>
       <c r="H54" s="2">
         <v>0</v>
@@ -2342,13 +2336,13 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>29.07232443926549</v>
+        <v>23.03426223551625</v>
       </c>
       <c r="E55">
         <v>5300</v>
       </c>
       <c r="G55">
-        <v>-18.95535193878692</v>
+        <v>0.7649479396638653</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -2359,13 +2353,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>29.76217726816773</v>
+        <v>23.67532550030654</v>
       </c>
       <c r="E56" s="2">
         <v>5400</v>
       </c>
       <c r="G56" s="2">
-        <v>-21.77802565445311</v>
+        <v>-1.996848631243644</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -2376,13 +2370,13 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>29.44278691163136</v>
+        <v>23.78346015101411</v>
       </c>
       <c r="E57">
         <v>5500</v>
       </c>
       <c r="G57">
-        <v>-20.471174791977</v>
+        <v>-2.462708904204618</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2393,13 +2387,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>29.84651132417257</v>
+        <v>23.78624119172401</v>
       </c>
       <c r="E58" s="2">
         <v>5600</v>
       </c>
       <c r="G58" s="2">
-        <v>-22.12309566539905</v>
+        <v>-2.474690044160679</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
@@ -2410,13 +2404,13 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>29.76194509308932</v>
+        <v>23.75771675344369</v>
       </c>
       <c r="E59">
         <v>5700</v>
       </c>
       <c r="G59">
-        <v>-21.77707566271022</v>
+        <v>-2.351802491314524</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2427,43 +2421,26 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>34.23176934232991</v>
+        <v>23.69933032256922</v>
       </c>
       <c r="E60" s="2">
         <v>5800</v>
       </c>
       <c r="G60" s="2">
-        <v>-40.06627430534797</v>
+        <v>-2.100265001283204</v>
       </c>
       <c r="H60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61">
-        <v>60</v>
-      </c>
       <c r="B61">
-        <v>34.40217024278832</v>
-      </c>
-      <c r="E61">
-        <v>5900</v>
+        <v>23.65545972831452</v>
       </c>
       <c r="G61">
-        <v>-40.76350438500883</v>
+        <v>-1.911263909766991</v>
       </c>
       <c r="H61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="B62">
-        <v>29.95937605115229</v>
-      </c>
-      <c r="G62">
-        <v>-22.58490474252993</v>
-      </c>
-      <c r="H62">
         <v>0</v>
       </c>
     </row>

</xml_diff>